<commit_message>
Added more cost info
</commit_message>
<xml_diff>
--- a/Hardware/BOM_epaper.xlsx
+++ b/Hardware/BOM_epaper.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Del\OneDrive\ePiPod\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drhat\OneDrive\ePiPod\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="203">
   <si>
     <t>Description</t>
   </si>
@@ -596,9 +596,6 @@
     <t>github.com/delhatch/PiPod_Zero2W</t>
   </si>
   <si>
-    <t>Not yet modified for the e-paper display</t>
-  </si>
-  <si>
     <t>Foam tape battery padding</t>
   </si>
   <si>
@@ -624,6 +621,18 @@
   </si>
   <si>
     <t>16-bit ADC</t>
+  </si>
+  <si>
+    <t>Bare PC board</t>
+  </si>
+  <si>
+    <t>PCBWay</t>
+  </si>
+  <si>
+    <t>https://www.pcbway.com/project/shareproject/ePaper_PiPod_MP3_music_player_a6adf3e1.html</t>
+  </si>
+  <si>
+    <t>See the link for ordering the PCB from PCBWay, or source files at github.</t>
   </si>
 </sst>
 </file>
@@ -685,7 +694,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -816,12 +825,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -876,16 +937,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -894,6 +945,37 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1176,24 +1258,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.1328125" customWidth="1"/>
+    <col min="2" max="2" width="19.46484375" customWidth="1"/>
+    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1212,14 +1294,14 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H1" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="H1" s="40" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1231,20 +1313,20 @@
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
       </c>
-      <c r="G2" s="38">
+      <c r="G2" s="34">
         <v>0.1</v>
       </c>
-      <c r="H2" s="39">
+      <c r="H2" s="35">
         <f>G2*F2</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1263,15 +1345,15 @@
       <c r="F3" s="4">
         <v>2</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="34">
         <v>0.1</v>
       </c>
-      <c r="H3" s="39">
-        <f t="shared" ref="H3:H53" si="0">G3*F3</f>
+      <c r="H3" s="35">
+        <f t="shared" ref="H3:H54" si="0">G3*F3</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -1290,15 +1372,15 @@
       <c r="F4" s="19">
         <v>12</v>
       </c>
-      <c r="G4" s="41">
+      <c r="G4" s="37">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="H4" s="42">
+      <c r="H4" s="38">
         <f t="shared" si="0"/>
         <v>0.42000000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1315,15 +1397,15 @@
       <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="34">
         <v>0.1</v>
       </c>
-      <c r="H5" s="39">
+      <c r="H5" s="35">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1340,15 +1422,15 @@
       <c r="F6" s="4">
         <v>5</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="34">
         <v>0.1</v>
       </c>
-      <c r="H6" s="39">
+      <c r="H6" s="35">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1365,15 +1447,15 @@
       <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="34">
         <v>0.1</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="35">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -1390,15 +1472,15 @@
       <c r="F8" s="4">
         <v>1</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G8" s="34">
         <v>0.1</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="35">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1415,15 +1497,15 @@
       <c r="F9" s="4">
         <v>1</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="34">
         <v>0.1</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="35">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -1440,15 +1522,15 @@
       <c r="F10" s="4">
         <v>1</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="34">
         <v>0.1</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="35">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1465,15 +1547,15 @@
       <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="34">
         <v>0.1</v>
       </c>
-      <c r="H11" s="39">
+      <c r="H11" s="35">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -1490,15 +1572,15 @@
       <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="34">
         <v>0.1</v>
       </c>
-      <c r="H12" s="39">
+      <c r="H12" s="35">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -1515,15 +1597,15 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G13" s="34">
         <v>0.27</v>
       </c>
-      <c r="H13" s="39">
+      <c r="H13" s="35">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="11" t="s">
         <v>43</v>
       </c>
@@ -1540,15 +1622,15 @@
       <c r="F14" s="11">
         <v>1</v>
       </c>
-      <c r="G14" s="38">
+      <c r="G14" s="34">
         <v>0.1</v>
       </c>
-      <c r="H14" s="39">
+      <c r="H14" s="35">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="13" t="s">
         <v>46</v>
       </c>
@@ -1567,15 +1649,15 @@
       <c r="F15" s="13">
         <v>2</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G15" s="34">
         <v>0.1</v>
       </c>
-      <c r="H15" s="39">
+      <c r="H15" s="35">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
@@ -1594,15 +1676,15 @@
       <c r="F16" s="1">
         <v>8</v>
       </c>
-      <c r="G16" s="38">
+      <c r="G16" s="34">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="35">
         <f t="shared" si="0"/>
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
@@ -1621,15 +1703,15 @@
       <c r="F17" s="1">
         <v>2</v>
       </c>
-      <c r="G17" s="38">
+      <c r="G17" s="34">
         <v>0.11</v>
       </c>
-      <c r="H17" s="39">
+      <c r="H17" s="35">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
@@ -1648,15 +1730,15 @@
       <c r="F18" s="1">
         <v>3</v>
       </c>
-      <c r="G18" s="38">
+      <c r="G18" s="34">
         <v>0.11</v>
       </c>
-      <c r="H18" s="39">
+      <c r="H18" s="35">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
@@ -1675,15 +1757,15 @@
       <c r="F19" s="1">
         <v>2</v>
       </c>
-      <c r="G19" s="38">
+      <c r="G19" s="34">
         <v>0.36</v>
       </c>
-      <c r="H19" s="39">
+      <c r="H19" s="35">
         <f t="shared" si="0"/>
         <v>0.72</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>67</v>
       </c>
@@ -1702,15 +1784,15 @@
       <c r="F20" s="1">
         <v>2</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="34">
         <v>0.68</v>
       </c>
-      <c r="H20" s="39">
+      <c r="H20" s="35">
         <f t="shared" si="0"/>
         <v>1.36</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>65</v>
       </c>
@@ -1729,15 +1811,15 @@
       <c r="F21" s="4">
         <v>2</v>
       </c>
-      <c r="G21" s="38">
+      <c r="G21" s="34">
         <v>0.1</v>
       </c>
-      <c r="H21" s="39">
+      <c r="H21" s="35">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>71</v>
       </c>
@@ -1751,20 +1833,20 @@
         <v>8</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F22" s="1">
         <v>11</v>
       </c>
-      <c r="G22" s="38">
+      <c r="G22" s="34">
         <v>0.183</v>
       </c>
-      <c r="H22" s="39">
+      <c r="H22" s="35">
         <f t="shared" si="0"/>
         <v>2.0129999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="11" t="s">
         <v>73</v>
       </c>
@@ -1783,15 +1865,15 @@
       <c r="F23" s="11">
         <v>4</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="34">
         <v>1.17</v>
       </c>
-      <c r="H23" s="39">
+      <c r="H23" s="35">
         <f t="shared" si="0"/>
         <v>4.68</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="13" t="s">
         <v>75</v>
       </c>
@@ -1810,15 +1892,15 @@
       <c r="F24" s="13">
         <v>2</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="34">
         <v>0.42</v>
       </c>
-      <c r="H24" s="39">
+      <c r="H24" s="35">
         <f t="shared" si="0"/>
         <v>0.84</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="11" t="s">
         <v>83</v>
       </c>
@@ -1837,15 +1919,15 @@
       <c r="F25" s="11">
         <v>3</v>
       </c>
-      <c r="G25" s="38">
+      <c r="G25" s="34">
         <v>0.34</v>
       </c>
-      <c r="H25" s="39">
+      <c r="H25" s="35">
         <f t="shared" si="0"/>
         <v>1.02</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="16" t="s">
         <v>88</v>
       </c>
@@ -1864,15 +1946,15 @@
       <c r="F26" s="16">
         <v>1</v>
       </c>
-      <c r="G26" s="38">
+      <c r="G26" s="34">
         <v>0.12</v>
       </c>
-      <c r="H26" s="39">
+      <c r="H26" s="35">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="13" t="s">
         <v>92</v>
       </c>
@@ -1891,15 +1973,15 @@
       <c r="F27" s="13">
         <v>1</v>
       </c>
-      <c r="G27" s="38">
+      <c r="G27" s="34">
         <v>1.97</v>
       </c>
-      <c r="H27" s="39">
+      <c r="H27" s="35">
         <f t="shared" si="0"/>
         <v>1.97</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="18" t="s">
         <v>96</v>
       </c>
@@ -1918,15 +2000,15 @@
       <c r="F28" s="18">
         <v>1</v>
       </c>
-      <c r="G28" s="41">
+      <c r="G28" s="37">
         <v>3.09</v>
       </c>
-      <c r="H28" s="42">
+      <c r="H28" s="38">
         <f t="shared" si="0"/>
         <v>3.09</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="18" t="s">
         <v>99</v>
       </c>
@@ -1945,15 +2027,15 @@
       <c r="F29" s="18">
         <v>1</v>
       </c>
-      <c r="G29" s="41">
+      <c r="G29" s="37">
         <v>0.78</v>
       </c>
-      <c r="H29" s="42">
+      <c r="H29" s="38">
         <f t="shared" si="0"/>
         <v>0.78</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A30" s="23" t="s">
         <v>102</v>
       </c>
@@ -1972,15 +2054,15 @@
       <c r="F30" s="23">
         <v>1</v>
       </c>
-      <c r="G30" s="41">
+      <c r="G30" s="37">
         <v>0.46</v>
       </c>
-      <c r="H30" s="42">
+      <c r="H30" s="38">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="13" t="s">
         <v>111</v>
       </c>
@@ -1999,15 +2081,15 @@
       <c r="F31" s="13">
         <v>1</v>
       </c>
-      <c r="G31" s="38">
+      <c r="G31" s="34">
         <v>1.41</v>
       </c>
-      <c r="H31" s="39">
+      <c r="H31" s="35">
         <f t="shared" si="0"/>
         <v>1.41</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -2026,15 +2108,15 @@
       <c r="F32" s="1">
         <v>1</v>
       </c>
-      <c r="G32" s="38">
+      <c r="G32" s="34">
         <v>1.2</v>
       </c>
-      <c r="H32" s="39">
+      <c r="H32" s="35">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>117</v>
       </c>
@@ -2053,15 +2135,15 @@
       <c r="F33" s="1">
         <v>1</v>
       </c>
-      <c r="G33" s="38">
+      <c r="G33" s="34">
         <v>0.34</v>
       </c>
-      <c r="H33" s="39">
+      <c r="H33" s="35">
         <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="11" t="s">
         <v>121</v>
       </c>
@@ -2080,15 +2162,15 @@
       <c r="F34" s="11">
         <v>1</v>
       </c>
-      <c r="G34" s="38">
+      <c r="G34" s="34">
         <v>0.34</v>
       </c>
-      <c r="H34" s="39">
+      <c r="H34" s="35">
         <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="13" t="s">
         <v>130</v>
       </c>
@@ -2107,15 +2189,15 @@
       <c r="F35" s="13">
         <v>3</v>
       </c>
-      <c r="G35" s="38">
+      <c r="G35" s="34">
         <v>0.51</v>
       </c>
-      <c r="H35" s="39">
+      <c r="H35" s="35">
         <f t="shared" si="0"/>
         <v>1.53</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>134</v>
       </c>
@@ -2134,15 +2216,15 @@
       <c r="F36" s="1">
         <v>5</v>
       </c>
-      <c r="G36" s="38">
+      <c r="G36" s="34">
         <v>0.627</v>
       </c>
-      <c r="H36" s="39">
+      <c r="H36" s="35">
         <f t="shared" si="0"/>
         <v>3.1349999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>138</v>
       </c>
@@ -2161,15 +2243,15 @@
       <c r="F37" s="1">
         <v>1</v>
       </c>
-      <c r="G37" s="38">
+      <c r="G37" s="34">
         <v>0.76</v>
       </c>
-      <c r="H37" s="39">
+      <c r="H37" s="35">
         <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>142</v>
       </c>
@@ -2188,15 +2270,15 @@
       <c r="F38" s="1">
         <v>2</v>
       </c>
-      <c r="G38" s="38">
+      <c r="G38" s="34">
         <v>0.5</v>
       </c>
-      <c r="H38" s="39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H38" s="35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="11" t="s">
         <v>143</v>
       </c>
@@ -2215,15 +2297,15 @@
       <c r="F39" s="11">
         <v>2</v>
       </c>
-      <c r="G39" s="38">
+      <c r="G39" s="34">
         <v>0.25</v>
       </c>
-      <c r="H39" s="39">
+      <c r="H39" s="35">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="25" t="s">
         <v>152</v>
       </c>
@@ -2242,16 +2324,16 @@
       <c r="F40" s="26">
         <v>1</v>
       </c>
-      <c r="G40" s="38">
+      <c r="G40" s="34">
         <f>6.7/50</f>
         <v>0.13400000000000001</v>
       </c>
-      <c r="H40" s="39">
+      <c r="H40" s="35">
         <f t="shared" si="0"/>
         <v>0.13400000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="28" t="s">
         <v>157</v>
       </c>
@@ -2270,20 +2352,20 @@
       <c r="F41" s="29">
         <v>1</v>
       </c>
-      <c r="G41" s="38">
+      <c r="G41" s="34">
         <v>1.19</v>
       </c>
-      <c r="H41" s="39">
+      <c r="H41" s="35">
         <f t="shared" si="0"/>
         <v>1.19</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="28" t="s">
         <v>159</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C42" s="29" t="s">
         <v>160</v>
@@ -2297,15 +2379,15 @@
       <c r="F42" s="29">
         <v>1</v>
       </c>
-      <c r="G42" s="38">
+      <c r="G42" s="34">
         <v>5.57</v>
       </c>
-      <c r="H42" s="39">
+      <c r="H42" s="35">
         <f t="shared" si="0"/>
         <v>5.57</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="28" t="s">
         <v>162</v>
       </c>
@@ -2324,15 +2406,15 @@
       <c r="F43" s="29">
         <v>1</v>
       </c>
-      <c r="G43" s="38">
+      <c r="G43" s="34">
         <v>4.79</v>
       </c>
-      <c r="H43" s="39">
+      <c r="H43" s="35">
         <f t="shared" si="0"/>
         <v>4.79</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="28" t="s">
         <v>165</v>
       </c>
@@ -2351,15 +2433,15 @@
       <c r="F44" s="29">
         <v>1</v>
       </c>
-      <c r="G44" s="38">
-        <v>1</v>
-      </c>
-      <c r="H44" s="39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G44" s="34">
+        <v>1</v>
+      </c>
+      <c r="H44" s="35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="28" t="s">
         <v>167</v>
       </c>
@@ -2378,15 +2460,15 @@
       <c r="F45" s="29">
         <v>1</v>
       </c>
-      <c r="G45" s="38">
+      <c r="G45" s="34">
         <v>1.21</v>
       </c>
-      <c r="H45" s="39">
+      <c r="H45" s="35">
         <f t="shared" si="0"/>
         <v>1.21</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A46" s="31" t="s">
         <v>170</v>
       </c>
@@ -2395,10 +2477,10 @@
       <c r="D46" s="31"/>
       <c r="E46" s="31"/>
       <c r="F46" s="31"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="39"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G46" s="34"/>
+      <c r="H46" s="35"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="25" t="s">
         <v>171</v>
       </c>
@@ -2413,178 +2495,189 @@
       <c r="F47" s="26">
         <v>1</v>
       </c>
-      <c r="G47" s="38">
+      <c r="G47" s="34">
         <v>9.9499999999999993</v>
       </c>
-      <c r="H47" s="39">
+      <c r="H47" s="35">
         <f t="shared" si="0"/>
         <v>9.9499999999999993</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="32" t="s">
         <v>174</v>
       </c>
       <c r="B48" s="33"/>
       <c r="C48" s="33"/>
       <c r="D48" s="33"/>
-      <c r="E48" t="s">
+      <c r="E48" s="29" t="s">
         <v>188</v>
       </c>
       <c r="F48" s="29">
         <v>1</v>
       </c>
-      <c r="G48" s="38">
+      <c r="G48" s="34">
         <v>15</v>
       </c>
-      <c r="H48" s="39">
+      <c r="H48" s="35">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="28" t="s">
+    <row r="49" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A49" s="41" t="s">
+        <v>199</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="F49" s="40">
+        <v>1</v>
+      </c>
+      <c r="G49" s="37">
+        <v>5</v>
+      </c>
+      <c r="H49" s="38">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A50" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="B49" s="29" t="s">
+      <c r="B50" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29" t="s">
+      <c r="C50" s="29"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="F49" s="34">
-        <v>1</v>
-      </c>
-      <c r="G49" s="38">
+      <c r="F50" s="29">
+        <v>1</v>
+      </c>
+      <c r="G50" s="34">
         <v>6.99</v>
       </c>
-      <c r="H49" s="39">
+      <c r="H50" s="35">
         <f t="shared" si="0"/>
         <v>6.99</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="28" t="s">
+    <row r="51" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="B50" s="35" t="s">
+      <c r="B51" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="C51" s="29"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="49" t="s">
+        <v>189</v>
+      </c>
+      <c r="F51" s="29">
+        <v>1</v>
+      </c>
+      <c r="G51" s="34">
+        <v>12.45</v>
+      </c>
+      <c r="H51" s="35">
+        <f t="shared" si="0"/>
+        <v>12.45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="B52" s="47"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="29">
+        <v>1</v>
+      </c>
+      <c r="G52" s="34">
+        <v>12.45</v>
+      </c>
+      <c r="H52" s="35">
+        <f t="shared" si="0"/>
+        <v>12.45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="B53" s="48"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="51"/>
+      <c r="F53" s="29">
+        <v>1</v>
+      </c>
+      <c r="G53" s="34">
+        <v>12.45</v>
+      </c>
+      <c r="H53" s="35">
+        <f t="shared" si="0"/>
+        <v>12.45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A54" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="F50" s="29">
-        <v>1</v>
-      </c>
-      <c r="G50" s="38">
-        <v>12.45</v>
-      </c>
-      <c r="H50" s="39">
-        <f t="shared" si="0"/>
-        <v>12.45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="B51" s="36"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="F51" s="29">
-        <v>1</v>
-      </c>
-      <c r="G51" s="38">
-        <v>12.45</v>
-      </c>
-      <c r="H51" s="39">
-        <f t="shared" si="0"/>
-        <v>12.45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="B52" s="37"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="F52" s="29">
-        <v>1</v>
-      </c>
-      <c r="G52" s="38">
-        <v>12.45</v>
-      </c>
-      <c r="H52" s="39">
-        <f t="shared" si="0"/>
-        <v>12.45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="6" t="s">
+      <c r="B54" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="C54" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="D54" s="43"/>
+      <c r="E54" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="F53" s="4">
-        <v>1</v>
-      </c>
-      <c r="G53" s="38">
+      <c r="F54" s="4">
+        <v>1</v>
+      </c>
+      <c r="G54" s="34">
         <f>18.36/20</f>
         <v>0.91799999999999993</v>
       </c>
-      <c r="H53" s="39">
+      <c r="H54" s="35">
         <f t="shared" si="0"/>
         <v>0.91799999999999993</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A55" s="44"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="44"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
-      <c r="H55" s="39">
-        <f>SUM(H2:H54)</f>
-        <v>114.95400000000001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H56" s="35">
+        <f>SUM(H2:H55)</f>
+        <v>119.95400000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2592,7 +2685,7 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2600,7 +2693,7 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -2608,7 +2701,7 @@
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -2616,9 +2709,18 @@
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B50:B52"/>
+  <mergeCells count="2">
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="E51:E53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>